<commit_message>
wrote a test script for testing aws instance boot times
</commit_message>
<xml_diff>
--- a/IaaSInstancePricingModels.xlsx
+++ b/IaaSInstancePricingModels.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozane\Downloads\Ongoing Courses\Thesis\Global-Server-Distribution-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF58AC2-9B51-4D21-9F93-2C95A56DD97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C1FCC-6718-4A06-BD5E-15A44A0534C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
   </bookViews>
   <sheets>
-    <sheet name="AWS Instance Prices" sheetId="1" r:id="rId1"/>
-    <sheet name="GCP Instance Prices" sheetId="2" r:id="rId2"/>
+    <sheet name="Cloud Instance Prices" sheetId="1" r:id="rId1"/>
+    <sheet name="Cloud Boot Duration Measurement" sheetId="2" r:id="rId2"/>
+    <sheet name="Cloud Latency Measurements" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Instances</t>
   </si>
@@ -130,6 +131,69 @@
   </si>
   <si>
     <t>c88</t>
+  </si>
+  <si>
+    <t>Test Number</t>
+  </si>
+  <si>
+    <t>Start Command</t>
+  </si>
+  <si>
+    <t>First Connection</t>
+  </si>
+  <si>
+    <t>17:19:04:285269400</t>
+  </si>
+  <si>
+    <t>17:19:18.640</t>
+  </si>
+  <si>
+    <t>17:24:57:749392400</t>
+  </si>
+  <si>
+    <t>17:25:11.798</t>
+  </si>
+  <si>
+    <t>17:28:45:079977400</t>
+  </si>
+  <si>
+    <t>17:28:59.814</t>
+  </si>
+  <si>
+    <t>17:31:53:475857500</t>
+  </si>
+  <si>
+    <t>17:32:05.635</t>
+  </si>
+  <si>
+    <t>17:33:42:036483700</t>
+  </si>
+  <si>
+    <t>17:33:54.202</t>
+  </si>
+  <si>
+    <t>17:35:33:582221700</t>
+  </si>
+  <si>
+    <t>17:35:46.783</t>
+  </si>
+  <si>
+    <t>17:37:35:797327600</t>
+  </si>
+  <si>
+    <t>17:37:49.004</t>
+  </si>
+  <si>
+    <t>17:40:11:165622400</t>
+  </si>
+  <si>
+    <t>17:40:24.876</t>
+  </si>
+  <si>
+    <t>17:41:24:234212900</t>
+  </si>
+  <si>
+    <t>17:41:37.564</t>
   </si>
 </sst>
 </file>
@@ -170,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -656,11 +720,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="7"/>
+      </top>
+      <bottom style="thick">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="7"/>
+      </top>
+      <bottom style="thick">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="5"/>
+      </right>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -781,6 +923,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1119,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9C580A-BFB7-41C3-AC61-7DB75EC9B287}">
   <dimension ref="B3:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5529182B-B29A-4EE2-8C40-13128FFD7E48}">
-  <dimension ref="B3:G12"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,164 +1795,395 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" customWidth="1"/>
+    <col min="5" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-    </row>
-    <row r="5" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="18" t="s">
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="46">
+        <v>1</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48">
+        <v>2</v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48">
+        <v>3</v>
+      </c>
+      <c r="J4" s="49"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>4</v>
       </c>
       <c r="C6" s="9">
         <v>8</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
+        <v>32</v>
+      </c>
+      <c r="C7" s="9">
+        <v>64</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
+        <v>64</v>
+      </c>
+      <c r="C8" s="9">
+        <v>128</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
+    </row>
+    <row r="15" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="45"/>
+      <c r="J15" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9">
+        <v>4</v>
+      </c>
+      <c r="C16" s="9">
+        <v>8</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E16" s="10">
         <v>0.14990000000000001</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10">
         <v>0.19309999999999999</v>
       </c>
-      <c r="G6" s="10">
+      <c r="I16" s="10"/>
+      <c r="J16" s="10">
         <v>0.18440000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+    <row r="17" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="9">
+        <v>32</v>
+      </c>
+      <c r="C17" s="9">
+        <v>64</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1.1993</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10">
+        <v>1.5451999999999999</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10">
+        <v>1.4751000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9">
+        <v>112</v>
+      </c>
+      <c r="C18" s="9">
+        <v>224</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="10">
+        <v>4.1977000000000002</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10">
+        <v>5.4081999999999999</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10">
+        <v>5.1631999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+    </row>
+    <row r="24" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
-        <v>16</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.29980000000000001</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0.38619999999999999</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.36880000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
-        <v>16</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="G24" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="9">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9">
+        <v>8</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="10" t="e">
+        <f>(E6+E16)/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G25" s="10" t="e">
+        <f>(H6+H16)/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H25" s="10" t="e">
+        <f>(J6+J16)/2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="9">
         <v>32</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0.59970000000000001</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0.77259999999999995</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0.73760000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
-        <v>32</v>
-      </c>
-      <c r="C9" s="9">
+      <c r="D26" s="9">
         <v>64</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1.1993</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1.5451999999999999</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1.4751000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
-        <v>56</v>
-      </c>
-      <c r="C10" s="9">
-        <v>112</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="10">
-        <v>2.0989</v>
-      </c>
-      <c r="F10" s="10">
-        <v>2.7040999999999999</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2.5815999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
-        <v>112</v>
-      </c>
-      <c r="C11" s="9">
-        <v>224</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="10">
-        <v>4.1977000000000002</v>
-      </c>
-      <c r="F11" s="10">
-        <v>5.4081999999999999</v>
-      </c>
-      <c r="G11" s="10">
-        <v>5.1631999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E26" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="10" t="e">
+        <f>(E7+E17)/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G26" s="10" t="e">
+        <f>(H7+H17)/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H26" s="10" t="e">
+        <f>(J7+J17)/2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="9">
+        <v>88</v>
+      </c>
+      <c r="D27" s="9">
+        <v>176</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="10" t="e">
+        <f>(E8+E18)/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G27" s="10" t="e">
+        <f>(H8+H18)/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H27" s="10" t="e">
+        <f>(J8+J18)/2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E4:G4"/>
+  <mergeCells count="9">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CB0833-D094-4001-B34A-3AF054B7A1B0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added the gcp scripts aswell
</commit_message>
<xml_diff>
--- a/IaaSInstancePricingModels.xlsx
+++ b/IaaSInstancePricingModels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozane\Downloads\Ongoing Courses\Thesis\Global-Server-Distribution-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C1FCC-6718-4A06-BD5E-15A44A0534C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB1E850-D3BB-461E-9DAF-96AC3E875AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud Instance Prices" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
   <si>
     <t>Instances</t>
   </si>
@@ -142,66 +142,152 @@
     <t>First Connection</t>
   </si>
   <si>
-    <t>17:19:04:285269400</t>
-  </si>
-  <si>
     <t>17:19:18.640</t>
   </si>
   <si>
-    <t>17:24:57:749392400</t>
-  </si>
-  <si>
     <t>17:25:11.798</t>
   </si>
   <si>
-    <t>17:28:45:079977400</t>
-  </si>
-  <si>
     <t>17:28:59.814</t>
   </si>
   <si>
-    <t>17:31:53:475857500</t>
-  </si>
-  <si>
     <t>17:32:05.635</t>
   </si>
   <si>
-    <t>17:33:42:036483700</t>
-  </si>
-  <si>
     <t>17:33:54.202</t>
   </si>
   <si>
-    <t>17:35:33:582221700</t>
-  </si>
-  <si>
     <t>17:35:46.783</t>
   </si>
   <si>
-    <t>17:37:35:797327600</t>
-  </si>
-  <si>
     <t>17:37:49.004</t>
   </si>
   <si>
-    <t>17:40:11:165622400</t>
-  </si>
-  <si>
     <t>17:40:24.876</t>
   </si>
   <si>
-    <t>17:41:24:234212900</t>
-  </si>
-  <si>
     <t>17:41:37.564</t>
+  </si>
+  <si>
+    <t>17:19:04:285</t>
+  </si>
+  <si>
+    <t>17:31:53:475</t>
+  </si>
+  <si>
+    <t>17:37:35:797</t>
+  </si>
+  <si>
+    <t>17:24:57:749</t>
+  </si>
+  <si>
+    <t>17:33:42:036</t>
+  </si>
+  <si>
+    <t>17:40:11:165</t>
+  </si>
+  <si>
+    <t>17:28:45:079</t>
+  </si>
+  <si>
+    <t>17:35:33:582</t>
+  </si>
+  <si>
+    <t>17:41:24:234</t>
+  </si>
+  <si>
+    <t>Average Boot Durations Per Type</t>
+  </si>
+  <si>
+    <t>Total Average</t>
+  </si>
+  <si>
+    <t>21:45:43:336</t>
+  </si>
+  <si>
+    <t>21:45:51.540</t>
+  </si>
+  <si>
+    <t>21:49:33:657</t>
+  </si>
+  <si>
+    <t>21:49:43.671</t>
+  </si>
+  <si>
+    <t>21:51:46:202</t>
+  </si>
+  <si>
+    <t>21:51:54.459</t>
+  </si>
+  <si>
+    <t>00:01:37:357</t>
+  </si>
+  <si>
+    <t>00:01:46.681</t>
+  </si>
+  <si>
+    <t>00:04:01:202</t>
+  </si>
+  <si>
+    <t>00:04:11.459</t>
+  </si>
+  <si>
+    <t>00:05:12:991</t>
+  </si>
+  <si>
+    <t>00:05:21.556</t>
+  </si>
+  <si>
+    <t>00:13:20:365</t>
+  </si>
+  <si>
+    <t>00:13:29.999</t>
+  </si>
+  <si>
+    <t>00:16:04:159</t>
+  </si>
+  <si>
+    <t>00:16:13.666</t>
+  </si>
+  <si>
+    <t>00:19:40:688</t>
+  </si>
+  <si>
+    <t>00:19:50.876</t>
+  </si>
+  <si>
+    <t>Theoretical Boot Duration</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Oregon(Seattle)</t>
+  </si>
+  <si>
+    <t>4ms</t>
+  </si>
+  <si>
+    <t>285ms</t>
+  </si>
+  <si>
+    <t>364ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="170" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -234,7 +320,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -798,11 +884,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6"/>
+      </right>
+      <top style="thick">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -883,6 +993,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -925,28 +1050,121 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1285,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9C580A-BFB7-41C3-AC61-7DB75EC9B287}">
   <dimension ref="B3:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,27 +1525,27 @@
   <sheetData>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="28" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="2"/>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="34" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="36"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="41"/>
     </row>
     <row r="5" spans="2:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
@@ -1616,16 +1834,16 @@
     <row r="12" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="31" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18" t="s">
@@ -1784,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5529182B-B29A-4EE2-8C40-13128FFD7E48}">
-  <dimension ref="B2:K28"/>
+  <dimension ref="A2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,379 +2016,889 @@
     <col min="5" max="7" width="27.7109375" customWidth="1"/>
     <col min="8" max="9" width="30.5703125" customWidth="1"/>
     <col min="10" max="10" width="33.28515625" customWidth="1"/>
+    <col min="11" max="11" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="28" t="s">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
-    </row>
-    <row r="4" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="37" t="s">
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="46">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="47">
         <v>1</v>
       </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48">
+      <c r="F4" s="48"/>
+      <c r="G4" s="49">
         <v>2</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48">
+      <c r="H4" s="48"/>
+      <c r="I4" s="49">
         <v>3</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4" s="50"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
       <c r="B5" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="61" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="29" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="31" t="s">
         <v>32</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
       <c r="B6" s="9">
         <v>4</v>
       </c>
       <c r="C6" s="9">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="I6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="9">
+        <f>((14.355)+(14.049)+(14.735))/3</f>
+        <v>14.379666666666665</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
       <c r="B7" s="9">
         <v>32</v>
       </c>
       <c r="C7" s="9">
         <v>64</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="63" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="K7" s="9">
+        <f>((12.16)+(12.166)+(13.201))/3</f>
+        <v>12.509</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
       <c r="B8" s="9">
         <v>64</v>
       </c>
       <c r="C8" s="9">
         <v>128</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="64" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="9">
+        <f>((13.207)+(13.711)+(13.33))/3</f>
+        <v>13.415999999999999</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
+        <f>(K6+K7+K8)/3</f>
+        <v>13.434888888888887</v>
+      </c>
+      <c r="L9" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="66"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="54">
+        <v>1</v>
+      </c>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55">
+        <v>2</v>
+      </c>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55">
+        <v>3</v>
+      </c>
+      <c r="J14" s="56"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
       <c r="B15" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+        <v>32</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="H15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="45"/>
+        <v>33</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>32</v>
+      </c>
       <c r="J15" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="K15" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
       <c r="B16" s="9">
         <v>4</v>
       </c>
       <c r="C16" s="9">
         <v>8</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="10">
-        <v>0.14990000000000001</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10">
-        <v>0.19309999999999999</v>
-      </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10">
-        <v>0.18440000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="9">
+        <f>((8.204)+(10.014)+(8.257))/3</f>
+        <v>8.8250000000000011</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
       <c r="B17" s="9">
         <v>32</v>
       </c>
       <c r="C17" s="9">
         <v>64</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="10">
-        <v>1.1993</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10">
-        <v>1.5451999999999999</v>
-      </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10">
-        <v>1.4751000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="9">
+        <f>((9.324)+(10.257)+(8.565))/3</f>
+        <v>9.3819999999999997</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
       <c r="B18" s="9">
+        <v>56</v>
+      </c>
+      <c r="C18" s="9">
         <v>112</v>
       </c>
-      <c r="C18" s="9">
-        <v>224</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="10">
-        <v>4.1977000000000002</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10">
-        <v>5.4081999999999999</v>
-      </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10">
-        <v>5.1631999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
-    </row>
-    <row r="24" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="9">
-        <v>4</v>
-      </c>
-      <c r="D25" s="9">
-        <v>8</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="10" t="e">
-        <f>(E6+E16)/2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G25" s="10" t="e">
-        <f>(H6+H16)/2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H25" s="10" t="e">
-        <f>(J6+J16)/2</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="9">
-        <v>32</v>
-      </c>
-      <c r="D26" s="9">
-        <v>64</v>
-      </c>
-      <c r="E26" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="10" t="e">
-        <f>(E7+E17)/2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G26" s="10" t="e">
-        <f>(H7+H17)/2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H26" s="10" t="e">
-        <f>(J7+J17)/2</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="9">
-        <v>88</v>
-      </c>
-      <c r="D27" s="9">
-        <v>176</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="10" t="e">
-        <f>(E8+E18)/2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G27" s="10" t="e">
-        <f>(H8+H18)/2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H27" s="10" t="e">
-        <f>(J8+J18)/2</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D18" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" s="9">
+        <f>((9.634)+(9.507)+(10.188))/3</f>
+        <v>9.7763333333333335</v>
+      </c>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9">
+        <f>(K16+K17+K18)/3</f>
+        <v>9.3277777777777775</v>
+      </c>
+      <c r="L19" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" s="75"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="78"/>
+      <c r="D25" s="57">
+        <f>(K9+K19)/2</f>
+        <v>11.381333333333332</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2178,12 +2906,285 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CB0833-D094-4001-B34A-3AF054B7A1B0}">
-  <dimension ref="A1"/>
+  <dimension ref="C6:V21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="83" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="84"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="84"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="P20" s="9"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="79"/>
+      <c r="T20" s="79"/>
+      <c r="U20" s="79"/>
+      <c r="V20" s="79"/>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished the gcp measurement tools
</commit_message>
<xml_diff>
--- a/IaaSInstancePricingModels.xlsx
+++ b/IaaSInstancePricingModels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozane\Downloads\Ongoing Courses\Thesis\Global-Server-Distribution-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB1E850-D3BB-461E-9DAF-96AC3E875AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE78614-2E19-42B3-AA15-D1C7F807CE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
+    <workbookView xWindow="22932" yWindow="-528" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud Instance Prices" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
   <si>
     <t>Instances</t>
   </si>
@@ -278,6 +278,69 @@
   </si>
   <si>
     <t>364ms</t>
+  </si>
+  <si>
+    <t>5ms</t>
+  </si>
+  <si>
+    <t>451ms</t>
+  </si>
+  <si>
+    <t>348ms</t>
+  </si>
+  <si>
+    <t>16ms</t>
+  </si>
+  <si>
+    <t>255ms</t>
+  </si>
+  <si>
+    <t>18ms</t>
+  </si>
+  <si>
+    <t>274ms</t>
+  </si>
+  <si>
+    <t>405ms</t>
+  </si>
+  <si>
+    <t>2ms</t>
+  </si>
+  <si>
+    <t>338ms</t>
+  </si>
+  <si>
+    <t>391ms</t>
+  </si>
+  <si>
+    <t>277ms</t>
+  </si>
+  <si>
+    <t>359ms</t>
+  </si>
+  <si>
+    <t>Approximate Average Latency</t>
+  </si>
+  <si>
+    <t>20ms</t>
+  </si>
+  <si>
+    <t>380ms</t>
+  </si>
+  <si>
+    <t>260ms</t>
+  </si>
+  <si>
+    <t>370ms</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>400ms</t>
+  </si>
+  <si>
+    <t>320ms</t>
   </si>
 </sst>
 </file>
@@ -286,8 +349,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="170" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -320,7 +383,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -908,11 +971,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="5"/>
+      </left>
+      <right style="thick">
+        <color theme="5"/>
+      </right>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5"/>
+      </left>
+      <right style="thick">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5"/>
+      </left>
+      <right style="thick">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1008,6 +1108,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1050,6 +1201,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1062,27 +1249,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1092,72 +1258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,6 +1265,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1525,27 +1634,27 @@
   <sheetData>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="33" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="2"/>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="39" t="s">
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="2:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
@@ -1834,16 +1943,16 @@
     <row r="12" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="36" t="s">
+      <c r="C17" s="61"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="55"/>
     </row>
     <row r="18" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18" t="s">
@@ -2042,14 +2151,14 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -2058,23 +2167,23 @@
     </row>
     <row r="4" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="47">
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="76">
         <v>1</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49">
+      <c r="F4" s="77"/>
+      <c r="G4" s="78">
         <v>2</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49">
+      <c r="H4" s="77"/>
+      <c r="I4" s="78">
         <v>3</v>
       </c>
-      <c r="J4" s="50"/>
+      <c r="J4" s="79"/>
       <c r="K4" s="28"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
@@ -2089,7 +2198,7 @@
       <c r="C5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="37" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -2110,7 +2219,7 @@
       <c r="J5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="34" t="s">
         <v>52</v>
       </c>
       <c r="L5" s="9"/>
@@ -2126,10 +2235,10 @@
       <c r="C6" s="9">
         <v>8</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="33" t="s">
         <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -2164,7 +2273,7 @@
       <c r="C7" s="9">
         <v>64</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="39" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -2202,7 +2311,7 @@
       <c r="C8" s="9">
         <v>128</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="40" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -2247,10 +2356,10 @@
         <f>(K6+K7+K8)/3</f>
         <v>13.434888888888887</v>
       </c>
-      <c r="L9" s="65" t="s">
+      <c r="L9" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="66"/>
+      <c r="M9" s="70"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
@@ -2310,14 +2419,14 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="69"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="68"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -2326,23 +2435,23 @@
     </row>
     <row r="14" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="54">
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="73">
         <v>1</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55">
+      <c r="F14" s="74"/>
+      <c r="G14" s="74">
         <v>2</v>
       </c>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55">
+      <c r="H14" s="74"/>
+      <c r="I14" s="74">
         <v>3</v>
       </c>
-      <c r="J14" s="56"/>
+      <c r="J14" s="75"/>
       <c r="K14" s="28"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -2357,7 +2466,7 @@
       <c r="C15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="41" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
@@ -2378,7 +2487,7 @@
       <c r="J15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="53" t="s">
+      <c r="K15" s="35" t="s">
         <v>52</v>
       </c>
       <c r="L15" s="9"/>
@@ -2394,7 +2503,7 @@
       <c r="C16" s="9">
         <v>8</v>
       </c>
-      <c r="D16" s="71" t="s">
+      <c r="D16" s="42" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -2432,7 +2541,7 @@
       <c r="C17" s="9">
         <v>64</v>
       </c>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="43" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -2470,7 +2579,7 @@
       <c r="C18" s="9">
         <v>112</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="44" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -2515,10 +2624,10 @@
         <f>(K16+K17+K18)/3</f>
         <v>9.3277777777777775</v>
       </c>
-      <c r="L19" s="74" t="s">
+      <c r="L19" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="M19" s="75"/>
+      <c r="M19" s="72"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
@@ -2595,7 +2704,7 @@
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="76"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2609,11 +2718,11 @@
     </row>
     <row r="25" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="78"/>
-      <c r="D25" s="57">
+      <c r="C25" s="65"/>
+      <c r="D25" s="36">
         <f>(K9+K19)/2</f>
         <v>11.381333333333332</v>
       </c>
@@ -2886,6 +2995,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E13:J13"/>
@@ -2894,11 +3008,6 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:J14"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2908,12 +3017,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CB0833-D094-4001-B34A-3AF054B7A1B0}">
   <dimension ref="C6:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.140625" customWidth="1"/>
@@ -2987,46 +3099,58 @@
     <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="80" t="s">
+      <c r="E10" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="82" t="s">
+      <c r="G10" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="80" t="s">
+      <c r="H10" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="81" t="s">
+      <c r="I10" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="82" t="s">
+      <c r="J10" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="80" t="s">
+      <c r="K10" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="81" t="s">
+      <c r="L10" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="M10" s="82" t="s">
+      <c r="M10" s="49" t="s">
         <v>73</v>
       </c>
       <c r="N10" s="9"/>
     </row>
     <row r="11" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="K11" s="9" t="s">
         <v>78</v>
       </c>
@@ -3040,35 +3164,73 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="N12" s="9"/>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
+      <c r="D13" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="N13" s="9"/>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -3163,12 +3325,12 @@
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.25">
       <c r="P20" s="9"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="79"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="79"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.25">
       <c r="P21" s="9"/>

</xml_diff>

<commit_message>
Started the request generator for the algorithm simulation
</commit_message>
<xml_diff>
--- a/IaaSInstancePricingModels.xlsx
+++ b/IaaSInstancePricingModels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozane\Downloads\Ongoing Courses\Thesis\Global-Server-Distribution-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE78614-2E19-42B3-AA15-D1C7F807CE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EFF299-FAA6-45E0-8D6B-46A70818433D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-528" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
+    <workbookView xWindow="22932" yWindow="-528" windowWidth="23256" windowHeight="12456" xr2:uid="{10F9E64B-FC94-4E4A-9C4C-BEE9657835AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud Instance Prices" sheetId="1" r:id="rId1"/>
@@ -1159,6 +1159,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1265,15 +1274,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1612,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9C580A-BFB7-41C3-AC61-7DB75EC9B287}">
   <dimension ref="B3:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,27 +1634,27 @@
   <sheetData>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="2"/>
-      <c r="J4" s="63" t="s">
+      <c r="J4" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="56" t="s">
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="57"/>
-      <c r="O4" s="58"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
@@ -1943,16 +1943,16 @@
     <row r="12" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="53" t="s">
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
     </row>
     <row r="18" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18" t="s">
@@ -2151,14 +2151,14 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="82"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -2167,23 +2167,23 @@
     </row>
     <row r="4" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="76">
+      <c r="C4" s="62"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="79">
         <v>1</v>
       </c>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78">
+      <c r="F4" s="80"/>
+      <c r="G4" s="81">
         <v>2</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="78">
+      <c r="H4" s="80"/>
+      <c r="I4" s="81">
         <v>3</v>
       </c>
-      <c r="J4" s="79"/>
+      <c r="J4" s="82"/>
       <c r="K4" s="28"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
@@ -2356,10 +2356,10 @@
         <f>(K6+K7+K8)/3</f>
         <v>13.434888888888887</v>
       </c>
-      <c r="L9" s="69" t="s">
+      <c r="L9" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="70"/>
+      <c r="M9" s="73"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
@@ -2419,14 +2419,14 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="68"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="71"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -2435,23 +2435,23 @@
     </row>
     <row r="14" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="73">
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="76">
         <v>1</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74">
+      <c r="F14" s="77"/>
+      <c r="G14" s="77">
         <v>2</v>
       </c>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74">
+      <c r="H14" s="77"/>
+      <c r="I14" s="77">
         <v>3</v>
       </c>
-      <c r="J14" s="75"/>
+      <c r="J14" s="78"/>
       <c r="K14" s="28"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -2624,10 +2624,10 @@
         <f>(K16+K17+K18)/3</f>
         <v>9.3277777777777775</v>
       </c>
-      <c r="L19" s="71" t="s">
+      <c r="L19" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="M19" s="72"/>
+      <c r="M19" s="75"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
@@ -2718,10 +2718,10 @@
     </row>
     <row r="25" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="65"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="36">
         <f>(K9+K19)/2</f>
         <v>11.381333333333332</v>
@@ -3017,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CB0833-D094-4001-B34A-3AF054B7A1B0}">
   <dimension ref="C6:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -3079,21 +3079,21 @@
     <row r="9" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="84"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="83" t="s">
+      <c r="F9" s="87"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="83" t="s">
+      <c r="I9" s="87"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="L9" s="84"/>
-      <c r="M9" s="85"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="88"/>
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3130,7 +3130,7 @@
     </row>
     <row r="11" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="50" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -3164,7 +3164,7 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
-      <c r="D12" s="87" t="s">
+      <c r="D12" s="51" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -3198,7 +3198,7 @@
     </row>
     <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="9"/>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="52" t="s">
         <v>93</v>
       </c>
       <c r="E13" s="9" t="s">

</xml_diff>